<commit_message>
Agrego resultados de pruebas de API con Postman, informes finales y README
</commit_message>
<xml_diff>
--- a/api_testing/casos_api.xlsx
+++ b/api_testing/casos_api.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29725"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayra\Desktop\ProyectoFinal-ChazarretaMayra\api_testing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B140A84-6E62-40F8-8F7A-48906793D4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,149 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+  <si>
+    <t>Testing de API</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Método</t>
+  </si>
+  <si>
+    <t>Endpoint</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Resultado esperado</t>
+  </si>
+  <si>
+    <t>API-01</t>
+  </si>
+  <si>
+    <t>API-02</t>
+  </si>
+  <si>
+    <t>API-03</t>
+  </si>
+  <si>
+    <t>API-04</t>
+  </si>
+  <si>
+    <t>API-05</t>
+  </si>
+  <si>
+    <t>API-06</t>
+  </si>
+  <si>
+    <t>API-07</t>
+  </si>
+  <si>
+    <t>API-08</t>
+  </si>
+  <si>
+    <t>API-09</t>
+  </si>
+  <si>
+    <t>API-10</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>/products</t>
+  </si>
+  <si>
+    <t>Listar todos los productos</t>
+  </si>
+  <si>
+    <t>Código 200, body con al menos 1 producto</t>
+  </si>
+  <si>
+    <t>/products/7</t>
+  </si>
+  <si>
+    <t>/users/8</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>/users</t>
+  </si>
+  <si>
+    <t>/products/2</t>
+  </si>
+  <si>
+    <t>/carts/3</t>
+  </si>
+  <si>
+    <t>/users/1</t>
+  </si>
+  <si>
+    <t>/carts/77</t>
+  </si>
+  <si>
+    <t>Trae solo el producto 7</t>
+  </si>
+  <si>
+    <t>Trae todos los productos</t>
+  </si>
+  <si>
+    <t>Trae solamente el usuario 8</t>
+  </si>
+  <si>
+    <t>Añade un producto</t>
+  </si>
+  <si>
+    <t>Añade un usuario</t>
+  </si>
+  <si>
+    <t>Actualiza el producto 2</t>
+  </si>
+  <si>
+    <t>Actualiza el carro 3</t>
+  </si>
+  <si>
+    <t>Actualiza el usuario 1</t>
+  </si>
+  <si>
+    <t>Consultar producto inexistente</t>
+  </si>
+  <si>
+    <t>Código 404 o body vacío</t>
+  </si>
+  <si>
+    <t>Código 200, body con el producto 7</t>
+  </si>
+  <si>
+    <t>Código 200, body con el usuario 8</t>
+  </si>
+  <si>
+    <t>Código 201</t>
+  </si>
+  <si>
+    <t>Código 200</t>
+  </si>
+  <si>
+    <t>Código 200, body con estructura JSON</t>
+  </si>
+  <si>
+    <t>/carts/1</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +174,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Abadi"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3850D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor rgb="FFD5A6BD"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,14 +235,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF3850D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -330,13 +542,231 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>